<commit_message>
Result saving in \results Implemented multi simulation mode for sequential simulation runs
</commit_message>
<xml_diff>
--- a/settings.xlsx
+++ b/settings.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcel\Documents\Semesterarbeit FTM\05 - Modell new\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E269970-35AF-4426-BC11-7B6325DB9E79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67F90E8D-2525-4C85-9E1C-E31C4AB83075}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{4448D773-169C-4529-85E3-C4726B86DDB4}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" activeTab="1" xr2:uid="{4448D773-169C-4529-85E3-C4726B86DDB4}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="150">
   <si>
     <t xml:space="preserve">Setting File for MG EV Optimization </t>
   </si>
@@ -481,6 +482,9 @@
   </si>
   <si>
     <t>rh_ch</t>
+  </si>
+  <si>
+    <t>go</t>
   </si>
 </sst>
 </file>
@@ -908,8 +912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67373682-B2FF-4762-AA78-C7C8B3272755}">
   <dimension ref="A1:D94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" outlineLevelRow="1" x14ac:dyDescent="0.45"/>
@@ -2030,4 +2034,1216 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0997C43F-5CD8-41C0-BECA-BB10C773F4E1}">
+  <dimension ref="A1:J95"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C98" sqref="C98"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:10" ht="25.5" x14ac:dyDescent="0.75">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="D1" s="8"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B2" s="2"/>
+      <c r="D2" s="8"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="5">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B11" s="2"/>
+      <c r="D11" s="8"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A13" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B13" s="2">
+        <v>48</v>
+      </c>
+      <c r="C13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A14" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B14" s="2">
+        <v>24</v>
+      </c>
+      <c r="C14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B15" s="2"/>
+      <c r="D15" s="8"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A17" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="6">
+        <v>38367</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A18" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="2">
+        <v>10</v>
+      </c>
+      <c r="C18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A19" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2">
+        <v>25</v>
+      </c>
+      <c r="C19" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A20" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B21" s="2"/>
+      <c r="D21" s="8"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A22" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A23" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="C23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A24" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="C24" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B25" s="2"/>
+      <c r="D25" s="8"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A26" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A27" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B27" s="2">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27" s="10"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A28" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" t="s">
+        <v>3</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="D29" s="8"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A30" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="7"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A31" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B31" s="2">
+        <v>1</v>
+      </c>
+      <c r="C31" t="s">
+        <v>3</v>
+      </c>
+      <c r="D31" s="8"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A32" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B32" s="2">
+        <v>1</v>
+      </c>
+      <c r="C32" t="s">
+        <v>3</v>
+      </c>
+      <c r="D32" s="8"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A33" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33" t="s">
+        <v>3</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A34" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B34" s="2">
+        <v>1.355</v>
+      </c>
+      <c r="C34" t="s">
+        <v>31</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A35" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35" s="2">
+        <v>0</v>
+      </c>
+      <c r="C35" t="s">
+        <v>33</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A36" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36" s="2">
+        <v>0</v>
+      </c>
+      <c r="C36" t="s">
+        <v>35</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A37" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37" s="2">
+        <v>20</v>
+      </c>
+      <c r="C37" t="s">
+        <v>19</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A38" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38" s="2">
+        <v>1</v>
+      </c>
+      <c r="C38" t="s">
+        <v>3</v>
+      </c>
+      <c r="D38" s="10" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A39" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39" s="5">
+        <v>100000</v>
+      </c>
+      <c r="C39" t="s">
+        <v>39</v>
+      </c>
+      <c r="D39" s="10" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B40" s="2"/>
+      <c r="D40" s="8"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A41" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="7"/>
+      <c r="I41" s="7"/>
+      <c r="J41" s="7"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A42" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42" s="2">
+        <v>1</v>
+      </c>
+      <c r="C42" t="s">
+        <v>3</v>
+      </c>
+      <c r="D42" s="8"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A43" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B43" s="2">
+        <v>1</v>
+      </c>
+      <c r="C43" t="s">
+        <v>3</v>
+      </c>
+      <c r="D43" s="8"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A44" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C44" t="s">
+        <v>3</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A45" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B45" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="C45" t="s">
+        <v>31</v>
+      </c>
+      <c r="D45" s="10" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A46" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B46" s="2">
+        <v>0</v>
+      </c>
+      <c r="C46" t="s">
+        <v>33</v>
+      </c>
+      <c r="D46" s="10" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A47" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B47" s="2">
+        <v>0</v>
+      </c>
+      <c r="C47" t="s">
+        <v>35</v>
+      </c>
+      <c r="D47" s="10" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A48" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B48" s="2">
+        <v>25</v>
+      </c>
+      <c r="C48" t="s">
+        <v>19</v>
+      </c>
+      <c r="D48" s="10" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A49" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B49" s="2">
+        <v>1</v>
+      </c>
+      <c r="C49" t="s">
+        <v>3</v>
+      </c>
+      <c r="D49" s="10" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A50" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B50" s="5">
+        <v>205000</v>
+      </c>
+      <c r="C50" t="s">
+        <v>39</v>
+      </c>
+      <c r="D50" s="10" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B51" s="2"/>
+      <c r="D51" s="8"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A52" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="7"/>
+      <c r="F52" s="7"/>
+      <c r="G52" s="7"/>
+      <c r="H52" s="7"/>
+      <c r="I52" s="7"/>
+      <c r="J52" s="7"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A53" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B53" s="2">
+        <v>1</v>
+      </c>
+      <c r="C53" t="s">
+        <v>3</v>
+      </c>
+      <c r="D53" s="8"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A54" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="B54" s="2">
+        <v>1</v>
+      </c>
+      <c r="C54" t="s">
+        <v>3</v>
+      </c>
+      <c r="D54" s="8"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A55" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B55" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="C55" t="s">
+        <v>31</v>
+      </c>
+      <c r="D55" s="10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A56" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B56" s="2">
+        <v>0</v>
+      </c>
+      <c r="C56" t="s">
+        <v>33</v>
+      </c>
+      <c r="D56" s="10" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A57" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B57" s="2">
+        <v>6.4999999999999997E-4</v>
+      </c>
+      <c r="C57" t="s">
+        <v>35</v>
+      </c>
+      <c r="D57" s="10" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A58" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B58" s="2">
+        <v>10</v>
+      </c>
+      <c r="C58" t="s">
+        <v>19</v>
+      </c>
+      <c r="D58" s="10" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A59" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B59" s="2">
+        <v>1</v>
+      </c>
+      <c r="C59" t="s">
+        <v>3</v>
+      </c>
+      <c r="D59" s="10" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A60" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B60" s="5">
+        <v>85000</v>
+      </c>
+      <c r="C60" t="s">
+        <v>39</v>
+      </c>
+      <c r="D60" s="10" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="D61" s="8"/>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A62" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B62" s="3"/>
+      <c r="C62" s="3"/>
+      <c r="D62" s="9"/>
+      <c r="E62" s="7"/>
+      <c r="F62" s="7"/>
+      <c r="G62" s="7"/>
+      <c r="H62" s="7"/>
+      <c r="I62" s="7"/>
+      <c r="J62" s="7"/>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A63" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B63" s="2">
+        <v>1</v>
+      </c>
+      <c r="C63" t="s">
+        <v>3</v>
+      </c>
+      <c r="D63" s="8"/>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A64" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B64" s="2">
+        <v>1</v>
+      </c>
+      <c r="C64" t="s">
+        <v>3</v>
+      </c>
+      <c r="D64" s="8"/>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A65" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B65" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="C65" t="s">
+        <v>35</v>
+      </c>
+      <c r="D65" s="10" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A66" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B66" s="2">
+        <v>0</v>
+      </c>
+      <c r="C66" t="s">
+        <v>63</v>
+      </c>
+      <c r="D66" s="10" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A67" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B67" s="2">
+        <v>0</v>
+      </c>
+      <c r="C67" t="s">
+        <v>35</v>
+      </c>
+      <c r="D67" s="10" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A68" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B68" s="2">
+        <v>10</v>
+      </c>
+      <c r="C68" t="s">
+        <v>19</v>
+      </c>
+      <c r="D68" s="10" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A69" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B69" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="C69" t="s">
+        <v>3</v>
+      </c>
+      <c r="D69" s="10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A70" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B70" s="2">
+        <v>0.85</v>
+      </c>
+      <c r="C70" t="s">
+        <v>3</v>
+      </c>
+      <c r="D70" s="10" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A71" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B71" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C71" t="s">
+        <v>69</v>
+      </c>
+      <c r="D71" s="10" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A72" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B72" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C72" t="s">
+        <v>69</v>
+      </c>
+      <c r="D72" s="10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A73" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B73" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="C73" t="s">
+        <v>3</v>
+      </c>
+      <c r="D73" s="10" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A74" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B74" s="2">
+        <v>0</v>
+      </c>
+      <c r="C74" t="s">
+        <v>3</v>
+      </c>
+      <c r="D74" s="10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A75" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B75" s="2">
+        <v>1</v>
+      </c>
+      <c r="C75" t="s">
+        <v>3</v>
+      </c>
+      <c r="D75" s="10" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A76" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B76" s="5">
+        <v>65000</v>
+      </c>
+      <c r="C76" t="s">
+        <v>74</v>
+      </c>
+      <c r="D76" s="10" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B77" s="2"/>
+      <c r="D77" s="8"/>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A78" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B78" s="3"/>
+      <c r="C78" s="3"/>
+      <c r="D78" s="9"/>
+      <c r="E78" s="7"/>
+      <c r="F78" s="7"/>
+      <c r="G78" s="7"/>
+      <c r="H78" s="7"/>
+      <c r="I78" s="7"/>
+      <c r="J78" s="7"/>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A79" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B79" s="2">
+        <v>1</v>
+      </c>
+      <c r="C79" t="s">
+        <v>3</v>
+      </c>
+      <c r="D79" s="8"/>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A80" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B80" s="2">
+        <v>1</v>
+      </c>
+      <c r="C80" t="s">
+        <v>3</v>
+      </c>
+      <c r="D80" s="8"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A81" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C81" t="s">
+        <v>3</v>
+      </c>
+      <c r="D81" s="8"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A82" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B82" s="2">
+        <v>0</v>
+      </c>
+      <c r="C82" t="s">
+        <v>3</v>
+      </c>
+      <c r="D82" s="10" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A83" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B83" s="2">
+        <v>10</v>
+      </c>
+      <c r="C83" t="s">
+        <v>3</v>
+      </c>
+      <c r="D83" s="10" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A84" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B84" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="C84" t="s">
+        <v>35</v>
+      </c>
+      <c r="D84" s="10" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A85" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B85" s="2">
+        <v>0</v>
+      </c>
+      <c r="C85" t="s">
+        <v>63</v>
+      </c>
+      <c r="D85" s="10" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A86" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B86" s="2">
+        <v>0</v>
+      </c>
+      <c r="C86" t="s">
+        <v>35</v>
+      </c>
+      <c r="D86" s="10" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A87" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B87" s="2">
+        <v>10</v>
+      </c>
+      <c r="C87" t="s">
+        <v>19</v>
+      </c>
+      <c r="D87" s="10" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A88" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B88" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C88" t="s">
+        <v>140</v>
+      </c>
+      <c r="D88" s="10" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A89" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B89" s="2">
+        <v>3600</v>
+      </c>
+      <c r="C89" t="s">
+        <v>39</v>
+      </c>
+      <c r="D89" s="10" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A90" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B90" s="2">
+        <v>3600</v>
+      </c>
+      <c r="C90" t="s">
+        <v>39</v>
+      </c>
+      <c r="D90" s="10" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A91" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B91" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="C91" t="s">
+        <v>3</v>
+      </c>
+      <c r="D91" s="10" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A92" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B92" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="C92" t="s">
+        <v>3</v>
+      </c>
+      <c r="D92" s="10" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A93" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B93" s="2">
+        <v>1</v>
+      </c>
+      <c r="C93" t="s">
+        <v>3</v>
+      </c>
+      <c r="D93" s="10" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A94" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B94" s="5">
+        <v>30000</v>
+      </c>
+      <c r="C94" t="s">
+        <v>74</v>
+      </c>
+      <c r="D94" s="10" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="D95" s="8"/>
+    </row>
+  </sheetData>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B42:B43 B53:B54 B63:B64 B79:B80" xr:uid="{B95B67B3-DEF2-4867-997A-087D5914723A}">
+      <formula1>"True, False, 0, 1"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{844786F1-6681-4547-83F8-7D3F1386351E}">
+      <formula1>"cbc, gplk, gurobi"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B82 B6:B7 B31:B32" xr:uid="{874DA9C7-A4E9-4C70-AF7D-FBB3DADB7F7D}">
+      <formula1>"False, True, 0, 1"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10" xr:uid="{7C9D1B52-D06A-4057-92E3-8E98FA1BC8D6}">
+      <formula1>"go, rh"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>